<commit_message>
Falta la parte 4 que es que lo pueda hacer correo
</commit_message>
<xml_diff>
--- a/Data/Archivos_Generados/No procesados.xlsx
+++ b/Data/Archivos_Generados/No procesados.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data\Archivos_Generados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\importante\Generacion-Correo-Equipo-4\Data\Archivos_Generados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9432A1-004A-49DA-972E-BA7302A0F4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3427DA2-F318-42E5-A82C-D8AEBB2976C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1866586A-C123-49AC-8CB0-3E3B0F048993}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1866586A-C123-49AC-8CB0-3E3B0F048993}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>